<commit_message>
08.12.2023 - them tai khoan quan ly sach
</commit_message>
<xml_diff>
--- a/data/user.xlsx
+++ b/data/user.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21D81EAA-36DF-41C7-BA07-520F5FE1DD7D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9B12589-F32C-4C94-B2B1-AE98C96240DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8925" yWindow="240" windowWidth="17670" windowHeight="14985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="199">
   <si>
     <t>name</t>
   </si>
@@ -611,6 +611,12 @@
   </si>
   <si>
     <t>sba_admin</t>
+  </si>
+  <si>
+    <t>Quản lý sách</t>
+  </si>
+  <si>
+    <t>sba_manager</t>
   </si>
 </sst>
 </file>
@@ -944,10 +950,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E97"/>
+  <dimension ref="A1:E98"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A98" sqref="A98"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1248,49 +1254,49 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>197</v>
+      </c>
+      <c r="B18" t="s">
+        <v>198</v>
+      </c>
+      <c r="C18">
+        <v>22</v>
+      </c>
+      <c r="D18">
+        <v>4</v>
+      </c>
+      <c r="E18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B19" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C18" s="2">
+      <c r="C19" s="2">
         <v>9</v>
       </c>
-      <c r="D18" s="2">
+      <c r="D19" s="2">
         <v>5</v>
       </c>
-      <c r="E18" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>39</v>
-      </c>
-      <c r="B19" t="s">
-        <v>40</v>
-      </c>
-      <c r="C19">
-        <v>22</v>
-      </c>
-      <c r="D19">
-        <v>5</v>
-      </c>
-      <c r="E19">
+      <c r="E19" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B20" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C20">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D20">
         <v>5</v>
@@ -1301,13 +1307,13 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B21" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C21">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D21">
         <v>5</v>
@@ -1318,13 +1324,13 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B22" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C22">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D22">
         <v>5</v>
@@ -1335,16 +1341,16 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B23" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C23">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D23">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E23">
         <v>1</v>
@@ -1352,13 +1358,13 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B24" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C24">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D24">
         <v>6</v>
@@ -1369,13 +1375,13 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B25" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C25">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D25">
         <v>6</v>
@@ -1384,49 +1390,49 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="2" t="s">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>51</v>
+      </c>
+      <c r="B26" t="s">
+        <v>52</v>
+      </c>
+      <c r="C26">
+        <v>28</v>
+      </c>
+      <c r="D26">
+        <v>6</v>
+      </c>
+      <c r="E26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="B27" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="C26" s="2">
-        <v>10</v>
-      </c>
-      <c r="D26" s="2">
+      <c r="C27" s="2">
+        <v>10</v>
+      </c>
+      <c r="D27" s="2">
         <v>7</v>
       </c>
-      <c r="E26" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>55</v>
-      </c>
-      <c r="B27" t="s">
-        <v>56</v>
-      </c>
-      <c r="C27">
-        <v>29</v>
-      </c>
-      <c r="D27">
-        <v>7</v>
-      </c>
-      <c r="E27">
+      <c r="E27" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B28" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C28">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D28">
         <v>7</v>
@@ -1437,13 +1443,13 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B29" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C29">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D29">
         <v>7</v>
@@ -1454,13 +1460,13 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B30" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C30">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D30">
         <v>7</v>
@@ -1471,13 +1477,13 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B31" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C31">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D31">
         <v>7</v>
@@ -1488,13 +1494,13 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B32" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C32">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D32">
         <v>7</v>
@@ -1505,13 +1511,13 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B33" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C33">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D33">
         <v>7</v>
@@ -1520,49 +1526,49 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="2" t="s">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>67</v>
+      </c>
+      <c r="B34" t="s">
+        <v>68</v>
+      </c>
+      <c r="C34">
+        <v>35</v>
+      </c>
+      <c r="D34">
+        <v>7</v>
+      </c>
+      <c r="E34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="B34" s="2" t="s">
+      <c r="B35" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="C34" s="2">
+      <c r="C35" s="2">
         <v>11</v>
       </c>
-      <c r="D34" s="2">
+      <c r="D35" s="2">
         <v>8</v>
       </c>
-      <c r="E34" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>71</v>
-      </c>
-      <c r="B35" t="s">
-        <v>72</v>
-      </c>
-      <c r="C35">
-        <v>36</v>
-      </c>
-      <c r="D35">
-        <v>8</v>
-      </c>
-      <c r="E35">
+      <c r="E35" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B36" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C36">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D36">
         <v>8</v>
@@ -1573,13 +1579,13 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B37" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C37">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D37">
         <v>8</v>
@@ -1590,13 +1596,13 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B38" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C38">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D38">
         <v>8</v>
@@ -1607,13 +1613,13 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B39" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C39">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D39">
         <v>8</v>
@@ -1624,13 +1630,13 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B40" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C40">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D40">
         <v>8</v>
@@ -1641,13 +1647,13 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B41" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C41">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D41">
         <v>8</v>
@@ -1658,13 +1664,13 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B42" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C42">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D42">
         <v>8</v>
@@ -1675,13 +1681,13 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B43" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C43">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D43">
         <v>8</v>
@@ -1692,13 +1698,13 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B44" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C44">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D44">
         <v>8</v>
@@ -1707,49 +1713,49 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="2" t="s">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>89</v>
+      </c>
+      <c r="B45" t="s">
+        <v>90</v>
+      </c>
+      <c r="C45">
+        <v>45</v>
+      </c>
+      <c r="D45">
+        <v>8</v>
+      </c>
+      <c r="E45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="B45" s="2" t="s">
+      <c r="B46" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="C45" s="2">
+      <c r="C46" s="2">
         <v>12</v>
       </c>
-      <c r="D45" s="2">
+      <c r="D46" s="2">
         <v>9</v>
       </c>
-      <c r="E45" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>93</v>
-      </c>
-      <c r="B46" t="s">
-        <v>94</v>
-      </c>
-      <c r="C46">
-        <v>45</v>
-      </c>
-      <c r="D46">
-        <v>9</v>
-      </c>
-      <c r="E46">
+      <c r="E46" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B47" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C47">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D47">
         <v>9</v>
@@ -1760,13 +1766,13 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B48" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C48">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D48">
         <v>9</v>
@@ -1777,13 +1783,13 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B49" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C49">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D49">
         <v>9</v>
@@ -1794,13 +1800,13 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B50" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C50">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D50">
         <v>9</v>
@@ -1811,13 +1817,13 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B51" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C51">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D51">
         <v>9</v>
@@ -1828,13 +1834,13 @@
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B52" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C52">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D52">
         <v>9</v>
@@ -1845,13 +1851,13 @@
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B53" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C53">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D53">
         <v>9</v>
@@ -1862,13 +1868,13 @@
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B54" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C54">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D54">
         <v>9</v>
@@ -1879,13 +1885,13 @@
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B55" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C55">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D55">
         <v>9</v>
@@ -1896,13 +1902,13 @@
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B56" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C56">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D56">
         <v>9</v>
@@ -1913,13 +1919,13 @@
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B57" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C57">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D57">
         <v>9</v>
@@ -1930,13 +1936,13 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B58" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C58">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D58">
         <v>9</v>
@@ -1947,13 +1953,13 @@
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B59" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C59">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D59">
         <v>9</v>
@@ -1964,13 +1970,13 @@
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B60" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C60">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D60">
         <v>9</v>
@@ -1981,13 +1987,13 @@
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B61" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C61">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D61">
         <v>9</v>
@@ -1998,13 +2004,13 @@
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B62" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C62">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D62">
         <v>9</v>
@@ -2015,13 +2021,13 @@
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B63" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C63">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D63">
         <v>9</v>
@@ -2032,13 +2038,13 @@
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B64" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C64">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D64">
         <v>9</v>
@@ -2049,13 +2055,13 @@
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B65" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C65">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D65">
         <v>9</v>
@@ -2066,13 +2072,13 @@
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B66" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C66">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D66">
         <v>9</v>
@@ -2083,13 +2089,13 @@
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B67" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C67">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D67">
         <v>9</v>
@@ -2098,49 +2104,49 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="2" t="s">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>135</v>
+      </c>
+      <c r="B68" t="s">
+        <v>136</v>
+      </c>
+      <c r="C68">
+        <v>66</v>
+      </c>
+      <c r="D68">
+        <v>9</v>
+      </c>
+      <c r="E68">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="B68" s="2" t="s">
+      <c r="B69" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="C68" s="2">
+      <c r="C69" s="2">
         <v>13</v>
       </c>
-      <c r="D68" s="2">
-        <v>10</v>
-      </c>
-      <c r="E68" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
-        <v>139</v>
-      </c>
-      <c r="B69" t="s">
-        <v>140</v>
-      </c>
-      <c r="C69">
-        <v>67</v>
-      </c>
-      <c r="D69">
-        <v>10</v>
-      </c>
-      <c r="E69">
+      <c r="D69" s="2">
+        <v>10</v>
+      </c>
+      <c r="E69" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B70" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C70">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D70">
         <v>10</v>
@@ -2151,13 +2157,13 @@
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B71" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C71">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D71">
         <v>10</v>
@@ -2168,13 +2174,13 @@
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B72" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C72">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D72">
         <v>10</v>
@@ -2185,13 +2191,13 @@
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B73" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C73">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D73">
         <v>10</v>
@@ -2202,13 +2208,13 @@
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B74" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C74">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D74">
         <v>10</v>
@@ -2219,13 +2225,13 @@
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B75" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C75">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D75">
         <v>10</v>
@@ -2236,13 +2242,13 @@
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B76" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C76">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D76">
         <v>10</v>
@@ -2253,13 +2259,13 @@
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B77" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C77">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D77">
         <v>10</v>
@@ -2270,13 +2276,13 @@
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B78" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C78">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D78">
         <v>10</v>
@@ -2287,13 +2293,13 @@
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B79" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C79">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D79">
         <v>10</v>
@@ -2304,13 +2310,13 @@
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B80" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C80">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D80">
         <v>10</v>
@@ -2321,13 +2327,13 @@
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B81" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C81">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D81">
         <v>10</v>
@@ -2338,13 +2344,13 @@
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B82" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C82">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D82">
         <v>10</v>
@@ -2355,13 +2361,13 @@
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B83" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C83">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D83">
         <v>10</v>
@@ -2372,13 +2378,13 @@
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B84" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C84">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D84">
         <v>10</v>
@@ -2389,13 +2395,13 @@
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B85" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C85">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D85">
         <v>10</v>
@@ -2406,13 +2412,13 @@
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B86" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C86">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D86">
         <v>10</v>
@@ -2423,13 +2429,13 @@
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B87" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C87">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D87">
         <v>10</v>
@@ -2440,13 +2446,13 @@
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B88" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C88">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D88">
         <v>10</v>
@@ -2457,13 +2463,13 @@
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B89" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C89">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D89">
         <v>10</v>
@@ -2474,13 +2480,13 @@
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B90" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C90">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D90">
         <v>10</v>
@@ -2491,13 +2497,13 @@
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B91" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C91">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D91">
         <v>10</v>
@@ -2508,13 +2514,13 @@
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B92" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C92">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D92">
         <v>10</v>
@@ -2525,13 +2531,13 @@
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B93" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C93">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D93">
         <v>10</v>
@@ -2542,13 +2548,13 @@
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B94" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C94">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D94">
         <v>10</v>
@@ -2559,13 +2565,13 @@
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B95" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C95">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D95">
         <v>10</v>
@@ -2576,13 +2582,13 @@
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B96" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C96">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D96">
         <v>10</v>
@@ -2593,18 +2599,35 @@
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
+        <v>193</v>
+      </c>
+      <c r="B97" t="s">
+        <v>194</v>
+      </c>
+      <c r="C97">
+        <v>94</v>
+      </c>
+      <c r="D97">
+        <v>10</v>
+      </c>
+      <c r="E97">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
         <v>195</v>
       </c>
-      <c r="B97" t="s">
+      <c r="B98" t="s">
         <v>196</v>
       </c>
-      <c r="C97">
+      <c r="C98">
         <v>95</v>
       </c>
-      <c r="D97">
+      <c r="D98">
         <v>4</v>
       </c>
-      <c r="E97">
+      <c r="E98">
         <v>3</v>
       </c>
     </row>

</xml_diff>